<commit_message>
Update geloofsonderrig infographic style and restore poem to music feature
</commit_message>
<xml_diff>
--- a/PredikantJaarboek-2026-02-16.xlsx
+++ b/PredikantJaarboek-2026-02-16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e20bb24acbfe553d/Documents/Websites/DraMekaarSeLaste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E585AACB-F353-495F-BAC5-D8BACC0640EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{E585AACB-F353-495F-BAC5-D8BACC0640EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D114364D-5D2A-4FBA-9411-F66EA12BE11D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7908" yWindow="7908" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -3624,9 +3624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>